<commit_message>
hoac pt(100) figs and code updates
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -16,31 +16,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Acetic acid43</t>
+  </si>
+  <si>
+    <t>Acetaldehyde</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Ketene</t>
+  </si>
+  <si>
     <t>H2</t>
   </si>
   <si>
+    <t>Acetic acid60</t>
+  </si>
+  <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>Ethylene</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>HOAc</t>
-  </si>
-  <si>
-    <t>Formaldehyde</t>
-  </si>
-  <si>
-    <t>CO</t>
   </si>
 </sst>
 </file>
@@ -398,13 +398,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,40 +432,266 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>557591.9939691033</v>
+        <v>-1</v>
       </c>
       <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>6.023226644740085e-07</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>1.344941710783223e-06</v>
+      </c>
+      <c r="I2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>-1</v>
-      </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-      <c r="F2">
-        <v>-1</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-      <c r="H2">
-        <v>-1</v>
-      </c>
-      <c r="I2">
-        <v>-1</v>
-      </c>
-      <c r="J2">
-        <v>168667.5673458686</v>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+      <c r="F3">
+        <v>8.662993879037748e-07</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>1.424802033287694e-06</v>
+      </c>
+      <c r="I3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>0.0004</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>2.79860466923858e-07</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+      <c r="H4">
+        <v>1.071084382567251e-06</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>0.0008</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>5.329421183453525e-07</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>9.715907029045017e-07</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>0.0012</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+      <c r="F6">
+        <v>5.73752101054891e-07</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>8.498520080187098e-07</v>
+      </c>
+      <c r="I6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>0.0015</v>
+      </c>
+      <c r="B7">
+        <v>-1</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>7.416994930621231e-07</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>1.291435777499689e-06</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>0.003</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>1.20699759654942e-06</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>2.102431208430838e-06</v>
+      </c>
+      <c r="I8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>0.004</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>7.401729158066803e-07</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>9.731101506668055e-07</v>
+      </c>
+      <c r="I9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>0.005</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>2.924680721579058e-06</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>2.263300604122058e-06</v>
+      </c>
+      <c r="I10">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates and restructuring of data
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
+    <t>Acetic acid43</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
     <t>H2</t>
   </si>
   <si>
+    <t>Ketene</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
     <t>Acetaldehyde</t>
   </si>
   <si>
-    <t>Ketene</t>
-  </si>
-  <si>
     <t>Acetic acid60</t>
   </si>
   <si>
-    <t>Acetic acid43</t>
-  </si>
-  <si>
     <t>CO2</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>CO</t>
   </si>
   <si>
     <t>L</t>
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,231 +438,260 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.083464453286985e-06</v>
+        <v>-1</v>
       </c>
       <c r="C2">
         <v>-1</v>
       </c>
       <c r="D2">
-        <v>-1</v>
+        <v>1.345079964297693e-06</v>
       </c>
       <c r="E2">
         <v>-1</v>
       </c>
       <c r="F2">
-        <v>-1</v>
+        <v>7.854158387545218e-07</v>
       </c>
       <c r="G2">
-        <v>1.554980978975796e-07</v>
+        <v>-1</v>
       </c>
       <c r="H2">
         <v>-1</v>
       </c>
       <c r="I2">
-        <v>9.712120091304113e-07</v>
+        <v>1.51051300016021e-07</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>7.201041036462561e-07</v>
+        <v>-1</v>
       </c>
       <c r="C3">
         <v>-1</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>1.424790176625913e-06</v>
       </c>
       <c r="E3">
         <v>-1</v>
       </c>
       <c r="F3">
-        <v>-1</v>
+        <v>9.668408433756081e-07</v>
       </c>
       <c r="G3">
-        <v>8.050020467037268e-08</v>
+        <v>-1</v>
       </c>
       <c r="H3">
         <v>-1</v>
       </c>
       <c r="I3">
-        <v>3.61648330298459e-07</v>
+        <v>1.545272978201269e-07</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>0.0008</v>
+        <v>0.0004</v>
       </c>
       <c r="B4">
-        <v>7.483021813215779e-07</v>
+        <v>-1</v>
       </c>
       <c r="C4">
         <v>-1</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>1.070725567250404e-06</v>
       </c>
       <c r="E4">
         <v>-1</v>
       </c>
       <c r="F4">
-        <v>-1</v>
+        <v>3.609250316013533e-07</v>
       </c>
       <c r="G4">
-        <v>9.344044552769178e-08</v>
+        <v>-1</v>
       </c>
       <c r="H4">
         <v>-1</v>
       </c>
       <c r="I4">
-        <v>5.336640796333482e-07</v>
+        <v>6.885662223673767e-08</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>0.0012</v>
+        <v>0.0008</v>
       </c>
       <c r="B5">
-        <v>7.879540027714759e-07</v>
+        <v>-1</v>
       </c>
       <c r="C5">
         <v>-1</v>
       </c>
       <c r="D5">
-        <v>-1</v>
+        <v>9.716292974881019e-07</v>
       </c>
       <c r="E5">
         <v>-1</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>5.344902859832635e-07</v>
       </c>
       <c r="G5">
-        <v>8.417929935577388e-08</v>
+        <v>-1</v>
       </c>
       <c r="H5">
         <v>-1</v>
       </c>
       <c r="I5">
-        <v>5.684189018519682e-07</v>
+        <v>8.347650509387418e-08</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>0.0015</v>
+        <v>0.0012</v>
       </c>
       <c r="B6">
-        <v>9.192003895734584e-07</v>
+        <v>-1</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>8.498638856125455e-07</v>
       </c>
       <c r="E6">
         <v>-1</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>5.684576476198015e-07</v>
       </c>
       <c r="G6">
-        <v>1.135456925614902e-07</v>
+        <v>-1</v>
       </c>
       <c r="H6">
         <v>-1</v>
       </c>
       <c r="I6">
-        <v>7.151620526440192e-07</v>
+        <v>8.346556882406874e-08</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <v>0.003</v>
+        <v>0.0015</v>
       </c>
       <c r="B7">
-        <v>1.630410973688728e-06</v>
+        <v>-1</v>
       </c>
       <c r="C7">
         <v>-1</v>
       </c>
       <c r="D7">
-        <v>-1</v>
+        <v>1.291442370793711e-06</v>
       </c>
       <c r="E7">
         <v>-1</v>
       </c>
       <c r="F7">
-        <v>-1</v>
+        <v>7.130362430638149e-07</v>
       </c>
       <c r="G7">
-        <v>2.080698336382226e-07</v>
+        <v>-1</v>
       </c>
       <c r="H7">
         <v>-1</v>
       </c>
       <c r="I7">
-        <v>1.40206836228861e-06</v>
+        <v>1.174080074705969e-07</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="B8">
-        <v>7.086782024812195e-07</v>
+        <v>-1</v>
       </c>
       <c r="C8">
         <v>-1</v>
       </c>
       <c r="D8">
-        <v>-1</v>
+        <v>2.102430672936632e-06</v>
       </c>
       <c r="E8">
         <v>-1</v>
       </c>
       <c r="F8">
-        <v>-1</v>
+        <v>1.393567697711225e-06</v>
       </c>
       <c r="G8">
-        <v>1.096219994754588e-07</v>
+        <v>-1</v>
       </c>
       <c r="H8">
         <v>-1</v>
       </c>
       <c r="I8">
-        <v>7.303533364785682e-07</v>
+        <v>1.5506199015438e-07</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
+        <v>0.004</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>9.732524784643293e-07</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+      <c r="F9">
+        <v>7.279948254386134e-07</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
+        <v>1.059777857182084e-07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
         <v>0.005</v>
       </c>
-      <c r="B9">
-        <v>1.561084042171577e-06</v>
-      </c>
-      <c r="C9">
-        <v>-1</v>
-      </c>
-      <c r="D9">
-        <v>-1</v>
-      </c>
-      <c r="E9">
-        <v>-1</v>
-      </c>
-      <c r="F9">
-        <v>-1</v>
-      </c>
-      <c r="G9">
-        <v>2.348697875058594e-07</v>
-      </c>
-      <c r="H9">
-        <v>-1</v>
-      </c>
-      <c r="I9">
-        <v>1.97022700499429e-06</v>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>2.262929135699318e-06</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>1.963475081997287e-06</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+      <c r="I10">
+        <v>2.289070786371638e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
figs for Ni paper
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -14,30 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Acetic acid43</t>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>CO</t>
   </si>
   <si>
     <t>Water</t>
   </si>
   <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Ketene</t>
-  </si>
-  <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>Acetaldehyde</t>
-  </si>
-  <si>
-    <t>Acetic acid60</t>
-  </si>
-  <si>
-    <t>CO2</t>
+    <t>HOAc</t>
   </si>
   <si>
     <t>L</t>
@@ -398,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -423,275 +414,405 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>7561327.622822704</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D2">
-        <v>1.345079964297693e-06</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E2">
         <v>-1</v>
       </c>
       <c r="F2">
-        <v>7.854158387545218e-07</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-      <c r="H2">
-        <v>-1</v>
-      </c>
-      <c r="I2">
-        <v>1.51051300016021e-07</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="B3">
-        <v>-1</v>
+        <v>16282164.97813578</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>108719233.339913</v>
       </c>
       <c r="D3">
-        <v>1.424790176625913e-06</v>
+        <v>18987260.75799712</v>
       </c>
       <c r="E3">
         <v>-1</v>
       </c>
       <c r="F3">
-        <v>9.668408433756081e-07</v>
-      </c>
-      <c r="G3">
-        <v>-1</v>
-      </c>
-      <c r="H3">
-        <v>-1</v>
-      </c>
-      <c r="I3">
-        <v>1.545272978201269e-07</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>0.0004</v>
+        <v>1.01</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>17787591.33748112</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D4">
-        <v>1.070725567250404e-06</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E4">
         <v>-1</v>
       </c>
       <c r="F4">
-        <v>3.609250316013533e-07</v>
-      </c>
-      <c r="G4">
-        <v>-1</v>
-      </c>
-      <c r="H4">
-        <v>-1</v>
-      </c>
-      <c r="I4">
-        <v>6.885662223673767e-08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>0.0008</v>
+        <v>1.04</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>16209052.55288416</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D5">
-        <v>9.716292974881019e-07</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E5">
         <v>-1</v>
       </c>
       <c r="F5">
-        <v>5.344902859832635e-07</v>
-      </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>-1</v>
-      </c>
-      <c r="I5">
-        <v>8.347650509387418e-08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>0.0012</v>
+        <v>1.3</v>
       </c>
       <c r="B6">
-        <v>-1</v>
+        <v>17872321.7534636</v>
       </c>
       <c r="C6">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D6">
-        <v>8.498638856125455e-07</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E6">
         <v>-1</v>
       </c>
       <c r="F6">
-        <v>5.684576476198015e-07</v>
-      </c>
-      <c r="G6">
-        <v>-1</v>
-      </c>
-      <c r="H6">
-        <v>-1</v>
-      </c>
-      <c r="I6">
-        <v>8.346556882406874e-08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>0.0015</v>
+        <v>1.5</v>
       </c>
       <c r="B7">
-        <v>-1</v>
+        <v>11521769.02845364</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D7">
-        <v>1.291442370793711e-06</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E7">
         <v>-1</v>
       </c>
       <c r="F7">
-        <v>7.130362430638149e-07</v>
-      </c>
-      <c r="G7">
-        <v>-1</v>
-      </c>
-      <c r="H7">
-        <v>-1</v>
-      </c>
-      <c r="I7">
-        <v>1.174080074705969e-07</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>0.003</v>
+        <v>1.8</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>11302843.50130033</v>
       </c>
       <c r="C8">
-        <v>-1</v>
+        <v>116738344.7276593</v>
       </c>
       <c r="D8">
-        <v>2.102430672936632e-06</v>
+        <v>20834017.68103584</v>
       </c>
       <c r="E8">
         <v>-1</v>
       </c>
       <c r="F8">
-        <v>1.393567697711225e-06</v>
-      </c>
-      <c r="G8">
-        <v>-1</v>
-      </c>
-      <c r="H8">
-        <v>-1</v>
-      </c>
-      <c r="I8">
-        <v>1.5506199015438e-07</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>0.004</v>
+        <v>2.5</v>
       </c>
       <c r="B9">
-        <v>-1</v>
+        <v>14221414.84596121</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>80137455.6064499</v>
       </c>
       <c r="D9">
-        <v>9.732524784643293e-07</v>
+        <v>11380037.01593464</v>
       </c>
       <c r="E9">
         <v>-1</v>
       </c>
       <c r="F9">
-        <v>7.279948254386134e-07</v>
-      </c>
-      <c r="G9">
-        <v>-1</v>
-      </c>
-      <c r="H9">
-        <v>-1</v>
-      </c>
-      <c r="I9">
-        <v>1.059777857182084e-07</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>0.005</v>
+        <v>3.2</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>14822320.3418464</v>
       </c>
       <c r="C10">
-        <v>-1</v>
+        <v>90371559.83988744</v>
       </c>
       <c r="D10">
-        <v>2.262929135699318e-06</v>
+        <v>12431833.00443093</v>
       </c>
       <c r="E10">
         <v>-1</v>
       </c>
       <c r="F10">
-        <v>1.963475081997287e-06</v>
-      </c>
-      <c r="G10">
-        <v>-1</v>
-      </c>
-      <c r="H10">
-        <v>-1</v>
-      </c>
-      <c r="I10">
-        <v>2.289070786371638e-07</v>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B11">
+        <v>17305511.7539629</v>
+      </c>
+      <c r="C11">
+        <v>53260479.12785688</v>
+      </c>
+      <c r="D11">
+        <v>8061486.0910345</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="B12">
+        <v>15539820.14622358</v>
+      </c>
+      <c r="C12">
+        <v>116117562.7339392</v>
+      </c>
+      <c r="D12">
+        <v>15123385.66730704</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="B13">
+        <v>11825985.62663229</v>
+      </c>
+      <c r="C13">
+        <v>116962796.7446434</v>
+      </c>
+      <c r="D13">
+        <v>16344229.97077986</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>3.86</v>
+      </c>
+      <c r="B14">
+        <v>9821637.440598581</v>
+      </c>
+      <c r="C14">
+        <v>112412969.9542895</v>
+      </c>
+      <c r="D14">
+        <v>18381504.65203911</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>4.9</v>
+      </c>
+      <c r="B15">
+        <v>16789610.85197198</v>
+      </c>
+      <c r="C15">
+        <v>132649852.1243531</v>
+      </c>
+      <c r="D15">
+        <v>17332358.19153716</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="B16">
+        <v>14595190.84249189</v>
+      </c>
+      <c r="C16">
+        <v>133421549.2734301</v>
+      </c>
+      <c r="D16">
+        <v>19107628.50224325</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="B17">
+        <v>16555300.36441313</v>
+      </c>
+      <c r="C17">
+        <v>121054749.0576133</v>
+      </c>
+      <c r="D17">
+        <v>17792521.86196001</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="B18">
+        <v>15567176.69019014</v>
+      </c>
+      <c r="C18">
+        <v>123463669.8591429</v>
+      </c>
+      <c r="D18">
+        <v>19631831.12930312</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="B19">
+        <v>15473100.96034378</v>
+      </c>
+      <c r="C19">
+        <v>118821528.4979442</v>
+      </c>
+      <c r="D19">
+        <v>19887520.68009411</v>
+      </c>
+      <c r="E19">
+        <v>-1</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="B20">
+        <v>16958663.53070267</v>
+      </c>
+      <c r="C20">
+        <v>128566464.3800524</v>
+      </c>
+      <c r="D20">
+        <v>17826434.91396135</v>
+      </c>
+      <c r="E20">
+        <v>-1</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="B21">
+        <v>16365996.77554328</v>
+      </c>
+      <c r="C21">
+        <v>119972532.8467586</v>
+      </c>
+      <c r="D21">
+        <v>19805851.48055682</v>
+      </c>
+      <c r="E21">
+        <v>-1</v>
+      </c>
+      <c r="F21">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated HOAc/Ni(110) areas for uptake
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -14,15 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>H2</t>
   </si>
   <si>
-    <t>CO</t>
+    <t>Water</t>
   </si>
   <si>
-    <t>Furfural</t>
+    <t>HOAc</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO</t>
   </si>
   <si>
     <t>L</t>
@@ -383,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -402,159 +408,311 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>39647.94090432831</v>
+        <v>99432864.00967157</v>
       </c>
       <c r="C2">
-        <v>53289.54006569384</v>
+        <v>517946.8848767537</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>67958.38511778528</v>
+      </c>
+      <c r="E2">
+        <v>7559296.938035149</v>
+      </c>
+      <c r="F2">
+        <v>5077998.739689221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>0.0025</v>
+        <v>0.12</v>
       </c>
       <c r="B3">
-        <v>71014.17082206754</v>
+        <v>123839430.9698689</v>
       </c>
       <c r="C3">
-        <v>134512.2513211424</v>
+        <v>392865.6101648219</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>1448068.281180765</v>
+      </c>
+      <c r="E3">
+        <v>16285203.05489251</v>
+      </c>
+      <c r="F3">
+        <v>13585008.49200085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>0.005</v>
+        <v>1.04</v>
       </c>
       <c r="B4">
-        <v>91951.3862600017</v>
+        <v>122436829.073636</v>
       </c>
       <c r="C4">
-        <v>225505.1516375042</v>
+        <v>404390.9086209311</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>4105228.491097312</v>
+      </c>
+      <c r="E4">
+        <v>16213893.11565916</v>
+      </c>
+      <c r="F4">
+        <v>13434788.10757477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>0.01</v>
+        <v>1.5</v>
       </c>
       <c r="B5">
-        <v>143400.444486012</v>
+        <v>98869495.51061505</v>
       </c>
       <c r="C5">
-        <v>369046.2101706367</v>
+        <v>654221.0024057372</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>87225.60784737561</v>
+      </c>
+      <c r="E5">
+        <v>11520319.95079422</v>
+      </c>
+      <c r="F5">
+        <v>7971459.861646389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>0.02</v>
+        <v>1.8</v>
       </c>
       <c r="B6">
-        <v>194364.4160084366</v>
+        <v>103458599.3286628</v>
       </c>
       <c r="C6">
-        <v>552385.8885022872</v>
+        <v>565537.5498243775</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>55055.75984406852</v>
+      </c>
+      <c r="E6">
+        <v>11301261.36477978</v>
+      </c>
+      <c r="F6">
+        <v>8063029.98399758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>0.03</v>
+        <v>2.5</v>
       </c>
       <c r="B7">
-        <v>220197.0923404225</v>
+        <v>120815990.679148</v>
       </c>
       <c r="C7">
-        <v>629180.5048302375</v>
+        <v>591018.4709477338</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>140340.5403203352</v>
+      </c>
+      <c r="E7">
+        <v>14224533.15584257</v>
+      </c>
+      <c r="F7">
+        <v>10600218.14778144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>0.04</v>
+        <v>3.2</v>
       </c>
       <c r="B8">
-        <v>234675.54978902</v>
+        <v>117327332.7438248</v>
       </c>
       <c r="C8">
-        <v>688906.6992083244</v>
+        <v>572378.1142500686</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>181001.7859671152</v>
+      </c>
+      <c r="E8">
+        <v>14824370.35927413</v>
+      </c>
+      <c r="F8">
+        <v>10838513.31413946</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>0.05</v>
+        <v>3.5</v>
       </c>
       <c r="B9">
-        <v>247010.151481444</v>
+        <v>115699576.6901286</v>
       </c>
       <c r="C9">
-        <v>713340.5935588621</v>
+        <v>454232.971138049</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>414761.8708728735</v>
+      </c>
+      <c r="E9">
+        <v>17303903.1349009</v>
+      </c>
+      <c r="F9">
+        <v>12872728.71279531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>0.06</v>
+        <v>3.6</v>
       </c>
       <c r="B10">
-        <v>246738.0007113309</v>
+        <v>127940382.8097512</v>
       </c>
       <c r="C10">
-        <v>737282.1589403527</v>
+        <v>446974.5344021593</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>232070.0411140699</v>
+      </c>
+      <c r="E10">
+        <v>15542286.01875807</v>
+      </c>
+      <c r="F10">
+        <v>11977008.39862336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>0.07000000000000001</v>
+        <v>4.9</v>
       </c>
       <c r="B11">
-        <v>226945.2524070228</v>
+        <v>131997818.9242533</v>
       </c>
       <c r="C11">
-        <v>673832.8131819105</v>
+        <v>400388.2611462406</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>524824.0145622536</v>
+      </c>
+      <c r="E11">
+        <v>16787424.83439553</v>
+      </c>
+      <c r="F11">
+        <v>13387017.79211063</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>0.1</v>
+        <v>6.3</v>
       </c>
       <c r="B12">
-        <v>247382.0137377641</v>
+        <v>128348734.352567</v>
       </c>
       <c r="C12">
-        <v>722444.333303143</v>
+        <v>262250.7352938735</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>461113.9672753855</v>
+      </c>
+      <c r="E12">
+        <v>14597034.15476643</v>
+      </c>
+      <c r="F12">
+        <v>12280105.25103936</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="B13">
+        <v>130262217.033169</v>
+      </c>
+      <c r="C13">
+        <v>312411.6691422397</v>
+      </c>
+      <c r="D13">
+        <v>1892970.045781083</v>
+      </c>
+      <c r="E13">
+        <v>16556193.38364927</v>
+      </c>
+      <c r="F13">
+        <v>13138063.60631272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="B14">
+        <v>122040816.6441483</v>
+      </c>
+      <c r="C14">
+        <v>245106.2026059856</v>
+      </c>
+      <c r="D14">
+        <v>840643.6479315368</v>
+      </c>
+      <c r="E14">
+        <v>15570791.38196047</v>
+      </c>
+      <c r="F14">
+        <v>12903431.32376256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="B15">
+        <v>124884999.5788654</v>
+      </c>
+      <c r="C15">
+        <v>260454.6925466568</v>
+      </c>
+      <c r="D15">
+        <v>650669.0681010915</v>
+      </c>
+      <c r="E15">
+        <v>15471984.68909211</v>
+      </c>
+      <c r="F15">
+        <v>12206096.30309541</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="B16">
+        <v>130525130.2219138</v>
+      </c>
+      <c r="C16">
+        <v>300211.2081272746</v>
+      </c>
+      <c r="D16">
+        <v>1696378.998010783</v>
+      </c>
+      <c r="E16">
+        <v>16368221.28626128</v>
+      </c>
+      <c r="F16">
+        <v>13519583.02790464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOAc fig updates and some gua updates too
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>HOAc</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
   <si>
     <t>H2</t>
   </si>
@@ -22,13 +31,19 @@
     <t>Water</t>
   </si>
   <si>
-    <t>HOAc</t>
-  </si>
-  <si>
-    <t>CO2</t>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>31-ol</t>
   </si>
   <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>27-eth</t>
+  </si>
+  <si>
+    <t>Formaldehyde</t>
   </si>
   <si>
     <t>L</t>
@@ -389,15 +404,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -414,305 +429,195 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>99432864.00967157</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>517946.8848767537</v>
+        <v>87862.51521948514</v>
       </c>
       <c r="D2">
-        <v>67958.38511778528</v>
+        <v>37464.94620965197</v>
       </c>
       <c r="E2">
-        <v>7559296.938035149</v>
+        <v>189196.67414461</v>
       </c>
       <c r="F2">
-        <v>5077998.739689221</v>
+        <v>862.8885020443796</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>6110.872070548702</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>123839430.9698689</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>392865.6101648219</v>
+        <v>901.3557252807543</v>
       </c>
       <c r="D3">
-        <v>1448068.281180765</v>
+        <v>5246.256548799547</v>
       </c>
       <c r="E3">
-        <v>16285203.05489251</v>
+        <v>64666.88147656654</v>
       </c>
       <c r="F3">
-        <v>13585008.49200085</v>
+        <v>463.2763694308545</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>5030.789028124547</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
-        <v>1.04</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>122436829.073636</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>404390.9086209311</v>
+        <v>355782.7421492958</v>
       </c>
       <c r="D4">
-        <v>4105228.491097312</v>
+        <v>282115.9197452329</v>
       </c>
       <c r="E4">
-        <v>16213893.11565916</v>
+        <v>1542838.083176483</v>
       </c>
       <c r="F4">
-        <v>13434788.10757477</v>
+        <v>969.8567210722971</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>6956.884398397181</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>98869495.51061505</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>654221.0024057372</v>
+        <v>70150.40613619333</v>
       </c>
       <c r="D5">
-        <v>87225.60784737561</v>
+        <v>70758.16227232706</v>
       </c>
       <c r="E5">
-        <v>11520319.95079422</v>
+        <v>226470.3478108241</v>
       </c>
       <c r="F5">
-        <v>7971459.861646389</v>
+        <v>375.1264307713633</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>5801.834539715176</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>103458599.3286628</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>565537.5498243775</v>
+        <v>20013.28768253774</v>
       </c>
       <c r="D6">
-        <v>55055.75984406852</v>
+        <v>33410.71622046847</v>
       </c>
       <c r="E6">
-        <v>11301261.36477978</v>
+        <v>189888.0074743556</v>
       </c>
       <c r="F6">
-        <v>8063029.98399758</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="B7">
-        <v>120815990.679148</v>
-      </c>
-      <c r="C7">
-        <v>591018.4709477338</v>
-      </c>
-      <c r="D7">
-        <v>140340.5403203352</v>
-      </c>
-      <c r="E7">
-        <v>14224533.15584257</v>
-      </c>
-      <c r="F7">
-        <v>10600218.14778144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="B8">
-        <v>117327332.7438248</v>
-      </c>
-      <c r="C8">
-        <v>572378.1142500686</v>
-      </c>
-      <c r="D8">
-        <v>181001.7859671152</v>
-      </c>
-      <c r="E8">
-        <v>14824370.35927413</v>
-      </c>
-      <c r="F8">
-        <v>10838513.31413946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="B9">
-        <v>115699576.6901286</v>
-      </c>
-      <c r="C9">
-        <v>454232.971138049</v>
-      </c>
-      <c r="D9">
-        <v>414761.8708728735</v>
-      </c>
-      <c r="E9">
-        <v>17303903.1349009</v>
-      </c>
-      <c r="F9">
-        <v>12872728.71279531</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="B10">
-        <v>127940382.8097512</v>
-      </c>
-      <c r="C10">
-        <v>446974.5344021593</v>
-      </c>
-      <c r="D10">
-        <v>232070.0411140699</v>
-      </c>
-      <c r="E10">
-        <v>15542286.01875807</v>
-      </c>
-      <c r="F10">
-        <v>11977008.39862336</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1">
-        <v>4.9</v>
-      </c>
-      <c r="B11">
-        <v>131997818.9242533</v>
-      </c>
-      <c r="C11">
-        <v>400388.2611462406</v>
-      </c>
-      <c r="D11">
-        <v>524824.0145622536</v>
-      </c>
-      <c r="E11">
-        <v>16787424.83439553</v>
-      </c>
-      <c r="F11">
-        <v>13387017.79211063</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1">
-        <v>6.3</v>
-      </c>
-      <c r="B12">
-        <v>128348734.352567</v>
-      </c>
-      <c r="C12">
-        <v>262250.7352938735</v>
-      </c>
-      <c r="D12">
-        <v>461113.9672753855</v>
-      </c>
-      <c r="E12">
-        <v>14597034.15476643</v>
-      </c>
-      <c r="F12">
-        <v>12280105.25103936</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1">
-        <v>7.6</v>
-      </c>
-      <c r="B13">
-        <v>130262217.033169</v>
-      </c>
-      <c r="C13">
-        <v>312411.6691422397</v>
-      </c>
-      <c r="D13">
-        <v>1892970.045781083</v>
-      </c>
-      <c r="E13">
-        <v>16556193.38364927</v>
-      </c>
-      <c r="F13">
-        <v>13138063.60631272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1">
-        <v>8.4</v>
-      </c>
-      <c r="B14">
-        <v>122040816.6441483</v>
-      </c>
-      <c r="C14">
-        <v>245106.2026059856</v>
-      </c>
-      <c r="D14">
-        <v>840643.6479315368</v>
-      </c>
-      <c r="E14">
-        <v>15570791.38196047</v>
-      </c>
-      <c r="F14">
-        <v>12903431.32376256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="B15">
-        <v>124884999.5788654</v>
-      </c>
-      <c r="C15">
-        <v>260454.6925466568</v>
-      </c>
-      <c r="D15">
-        <v>650669.0681010915</v>
-      </c>
-      <c r="E15">
-        <v>15471984.68909211</v>
-      </c>
-      <c r="F15">
-        <v>12206096.30309541</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1">
-        <v>9.6</v>
-      </c>
-      <c r="B16">
-        <v>130525130.2219138</v>
-      </c>
-      <c r="C16">
-        <v>300211.2081272746</v>
-      </c>
-      <c r="D16">
-        <v>1696378.998010783</v>
-      </c>
-      <c r="E16">
-        <v>16368221.28626128</v>
-      </c>
-      <c r="F16">
-        <v>13519583.02790464</v>
+        <v>518.7748801483344</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>6602.331451791789</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update init info with some masses and H2 saturation on Pt
</commit_message>
<xml_diff>
--- a/plotTPD_data programs/Acetic Acid Area_output.xlsx
+++ b/plotTPD_data programs/Acetic Acid Area_output.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Formaldehyde</t>
+    <t>GUA</t>
   </si>
   <si>
-    <t>L</t>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
   <si>
     <t>H2</t>
@@ -28,19 +31,7 @@
     <t>CO</t>
   </si>
   <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>Ethylene</t>
-  </si>
-  <si>
-    <t>HOAc</t>
-  </si>
-  <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>Water</t>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -398,13 +389,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,20 +414,8 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -444,25 +426,93 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>295787.0685278159</v>
+        <v>2353.529330162142</v>
       </c>
       <c r="E2">
-        <v>73388.10136466507</v>
+        <v>272561.5825838298</v>
       </c>
       <c r="F2">
-        <v>201542.0039680531</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1293.72548630566</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>9735.564846577565</v>
+        <v>391835.4054309646</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2513.069710310881</v>
+      </c>
+      <c r="E3">
+        <v>100908.4278142457</v>
+      </c>
+      <c r="F3">
+        <v>216842.3500618415</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2513.069710310881</v>
+      </c>
+      <c r="E4">
+        <v>335747.7936134483</v>
+      </c>
+      <c r="F4">
+        <v>204189.8259181912</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2513.069710310881</v>
+      </c>
+      <c r="E5">
+        <v>44716.4143642417</v>
+      </c>
+      <c r="F5">
+        <v>198496.9576079197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2513.069710310881</v>
+      </c>
+      <c r="E6">
+        <v>44295.81448838354</v>
+      </c>
+      <c r="F6">
+        <v>168471.5104367869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>